<commit_message>
Added first plots in results analysis
</commit_message>
<xml_diff>
--- a/test_results/08_08_127.xlsx
+++ b/test_results/08_08_127.xlsx
@@ -201,7 +201,7 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>F</t>
+    <t>Female</t>
   </si>
   <si>
     <t>Alcune volte un po' indecisa ma in generale abbastanza sicura</t>
@@ -216,7 +216,7 @@
     <t>Reverberation</t>
   </si>
   <si>
-    <t>Intermedio</t>
+    <t>Intermediate</t>
   </si>
   <si>
     <t>No problemi VR.</t>
@@ -228,7 +228,7 @@
     <t>VR</t>
   </si>
   <si>
-    <t>Nessuno</t>
+    <t>None</t>
   </si>
   <si>
     <t>Impairment</t>

</xml_diff>